<commit_message>
Update Self perception Inventory.xlsx
</commit_message>
<xml_diff>
--- a/Matériel/Self perception Inventory.xlsx
+++ b/Matériel/Self perception Inventory.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xavier\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elischerrer\Documents\GitHub\ICT-306\Matériel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3621AA-F876-4FEA-970F-1ED0D05D366B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
     <sheet name="Questionnaire" sheetId="1" r:id="rId2"/>
     <sheet name="Grille d'évaluation" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1335,7 +1334,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2056,28 +2055,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2790,23 +2789,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2842,23 +2824,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3034,7 +2999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3075,11 +3040,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3104,19 +3069,25 @@
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -3128,25 +3099,33 @@
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -3154,7 +3133,7 @@
       </c>
       <c r="B12">
         <f>SUM(B4:B11)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3169,49 +3148,65 @@
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -3219,7 +3214,7 @@
       </c>
       <c r="B23">
         <f>SUM(B15:B22)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3234,49 +3229,65 @@
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="5"/>
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
@@ -3284,7 +3295,7 @@
       </c>
       <c r="B34">
         <f>SUM(B26:B33)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3299,49 +3310,65 @@
       <c r="A37" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="5"/>
+      <c r="B37" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="5"/>
+      <c r="B39" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="5"/>
+      <c r="B40" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="5"/>
+      <c r="B41" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="5"/>
+      <c r="B42" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="5"/>
+      <c r="B43" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="5"/>
+      <c r="B44" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -3349,7 +3376,7 @@
       </c>
       <c r="B45">
         <f>SUM(B37:B44)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3364,49 +3391,65 @@
       <c r="A48" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="5"/>
+      <c r="B49" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="5"/>
+      <c r="B50" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="5"/>
+      <c r="B51" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="5"/>
+      <c r="B52" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B53" s="5"/>
+      <c r="B53" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="5"/>
+      <c r="B54" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B55" s="5"/>
+      <c r="B55" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
@@ -3414,7 +3457,7 @@
       </c>
       <c r="B56">
         <f>SUM(B48:B55)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3429,49 +3472,65 @@
       <c r="A59" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B59" s="5"/>
+      <c r="B59" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="5"/>
+      <c r="B60" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B61" s="5"/>
+      <c r="B61" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B62" s="5"/>
+      <c r="B62" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B63" s="5"/>
+      <c r="B63" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B64" s="5"/>
+      <c r="B64" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B65" s="5"/>
+      <c r="B65" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B66" s="5"/>
+      <c r="B66" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
@@ -3479,7 +3538,7 @@
       </c>
       <c r="B67">
         <f>SUM(B59:B66)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3494,49 +3553,65 @@
       <c r="A70" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B70" s="5"/>
+      <c r="B70" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B71" s="5"/>
+      <c r="B71" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B72" s="5"/>
+      <c r="B72" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B73" s="5"/>
+      <c r="B73" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B74" s="5"/>
+      <c r="B74" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B75" s="5"/>
+      <c r="B75" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B76" s="5"/>
+      <c r="B76" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B77" s="5"/>
+      <c r="B77" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
@@ -3544,7 +3619,7 @@
       </c>
       <c r="B78">
         <f>SUM(B70:B77)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3564,14 +3639,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3706,14 +3781,14 @@
       </c>
       <c r="C5" s="15">
         <f>Questionnaire!B9</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>78</v>
       </c>
       <c r="E5" s="15">
         <f>Questionnaire!B6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>79</v>
@@ -3734,14 +3809,14 @@
       </c>
       <c r="K5" s="15">
         <f>Questionnaire!B11</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5" s="14" t="s">
         <v>82</v>
       </c>
       <c r="M5" s="15">
         <f>Questionnaire!B10</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N5" s="14" t="s">
         <v>83</v>
@@ -3755,11 +3830,11 @@
       </c>
       <c r="Q5" s="15">
         <f>Questionnaire!B8</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R5" s="16">
         <f t="shared" ref="R5:R11" si="0">SUM(B5:Q5)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
@@ -3771,42 +3846,42 @@
       </c>
       <c r="C6" s="19">
         <f>Questionnaire!B19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>82</v>
       </c>
       <c r="E6" s="19">
         <f>Questionnaire!B21</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>78</v>
       </c>
       <c r="G6" s="19">
         <f>Questionnaire!B17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>83</v>
       </c>
       <c r="I6" s="19">
         <f>Questionnaire!B16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="18" t="s">
         <v>80</v>
       </c>
       <c r="K6" s="19">
         <f>Questionnaire!B18</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L6" s="18" t="s">
         <v>79</v>
       </c>
       <c r="M6" s="19">
         <f>Questionnaire!B15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="18" t="s">
         <v>77</v>
@@ -3824,7 +3899,7 @@
       </c>
       <c r="R6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
@@ -3836,14 +3911,14 @@
       </c>
       <c r="C7" s="19">
         <f>Questionnaire!B28</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>80</v>
       </c>
       <c r="E7" s="19">
         <f>Questionnaire!B29</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>77</v>
@@ -3857,39 +3932,39 @@
       </c>
       <c r="I7" s="19">
         <f>Questionnaire!B26</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>82</v>
       </c>
       <c r="K7" s="19">
         <f>Questionnaire!B32</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L7" s="18" t="s">
         <v>81</v>
       </c>
       <c r="M7" s="19">
         <f>Questionnaire!B33</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="18" t="s">
         <v>84</v>
       </c>
       <c r="O7" s="19">
         <f>Questionnaire!B30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="18" t="s">
         <v>83</v>
       </c>
       <c r="Q7" s="19">
         <f>Questionnaire!B27</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
@@ -3901,7 +3976,7 @@
       </c>
       <c r="C8" s="19">
         <f>Questionnaire!B38</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>84</v>
@@ -3922,14 +3997,14 @@
       </c>
       <c r="I8" s="19">
         <f>Questionnaire!B44</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>78</v>
       </c>
       <c r="K8" s="19">
         <f>Questionnaire!B39</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L8" s="18" t="s">
         <v>80</v>
@@ -3950,11 +4025,11 @@
       </c>
       <c r="Q8" s="19">
         <f>Questionnaire!B42</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
@@ -3966,14 +4041,14 @@
       </c>
       <c r="C9" s="19">
         <f>Questionnaire!B51</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>81</v>
       </c>
       <c r="E9" s="19">
         <f>Questionnaire!B55</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>84</v>
@@ -3994,14 +4069,14 @@
       </c>
       <c r="K9" s="19">
         <f>Questionnaire!B48</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L9" s="18" t="s">
         <v>83</v>
       </c>
       <c r="M9" s="19">
         <f>Questionnaire!B49</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N9" s="18" t="s">
         <v>78</v>
@@ -4019,7 +4094,7 @@
       </c>
       <c r="R9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
@@ -4031,14 +4106,14 @@
       </c>
       <c r="C10" s="19">
         <f>Questionnaire!B65</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>79</v>
       </c>
       <c r="E10" s="19">
         <f>Questionnaire!B59</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>81</v>
@@ -4052,28 +4127,28 @@
       </c>
       <c r="I10" s="19">
         <f>Questionnaire!B61</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="18" t="s">
         <v>84</v>
       </c>
       <c r="K10" s="19">
         <f>Questionnaire!B63</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" s="18" t="s">
         <v>77</v>
       </c>
       <c r="M10" s="19">
         <f>Questionnaire!B64</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="18" t="s">
         <v>83</v>
       </c>
       <c r="O10" s="19">
         <f>Questionnaire!B60</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P10" s="18" t="s">
         <v>80</v>
@@ -4084,7 +4159,7 @@
       </c>
       <c r="R10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4096,14 +4171,14 @@
       </c>
       <c r="C11" s="22">
         <f>Questionnaire!B70</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>77</v>
       </c>
       <c r="E11" s="22">
         <f>Questionnaire!B75</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="21" t="s">
         <v>80</v>
@@ -4124,14 +4199,14 @@
       </c>
       <c r="K11" s="22">
         <f>Questionnaire!B71</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="21" t="s">
         <v>84</v>
       </c>
       <c r="M11" s="22">
         <f>Questionnaire!B74</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N11" s="21" t="s">
         <v>81</v>
@@ -4145,11 +4220,11 @@
       </c>
       <c r="Q11" s="22">
         <f>Questionnaire!B72</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4159,42 +4234,42 @@
       <c r="B12" s="24"/>
       <c r="C12" s="25">
         <f>SUM(C5:C11)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="25">
         <f>SUM(E5:E11)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F12" s="24"/>
       <c r="G12" s="25">
         <f>SUM(G5:G11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="24"/>
       <c r="I12" s="25">
         <f>SUM(I5:I11)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="25">
         <f>SUM(K5:K11)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="L12" s="24"/>
       <c r="M12" s="25">
         <f>SUM(M5:M11)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N12" s="24"/>
       <c r="O12" s="25">
         <f>SUM(O5:O11)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P12" s="24"/>
       <c r="Q12" s="25">
         <f>SUM(Q5:Q11)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -4233,6 +4308,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
@@ -4242,15 +4326,6 @@
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4508,6 +4583,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EACDE16C-130D-4E5E-84A8-656A0A274BCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2C8B3FA-527F-4218-A6C9-399161443A91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4515,14 +4598,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
     <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
     <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EACDE16C-130D-4E5E-84A8-656A0A274BCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>